<commit_message>
4/24 added back in attraction trials (binary and trinary) to choice-only experiment
</commit_message>
<xml_diff>
--- a/design_choice_only/stim_crit.xlsx
+++ b/design_choice_only/stim_crit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/ce_rating/design_choice_only/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DC6B0F-886B-CE4F-BD6B-EFED4B304704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E914538E-EF5D-A847-B5E4-38339E67C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="500" windowWidth="24640" windowHeight="15100" xr2:uid="{83BDC93F-3B75-2E41-8B80-1829027D4291}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
   <si>
     <t>t_high</t>
   </si>
@@ -62,16 +62,22 @@
     <t>repulsion_2</t>
   </si>
   <si>
+    <t>attraction_1</t>
+  </si>
+  <si>
+    <t>attraction_2</t>
+  </si>
+  <si>
     <t>d1</t>
   </si>
   <si>
     <t>d2</t>
   </si>
   <si>
+    <t>trinary</t>
+  </si>
+  <si>
     <t>set</t>
-  </si>
-  <si>
-    <t>trinary</t>
   </si>
   <si>
     <t>binary</t>
@@ -460,17 +466,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D09608-67B5-B54A-8956-53E291167A46}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -479,18 +485,18 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -508,9 +514,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -528,9 +534,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -548,9 +554,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -568,9 +574,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -588,9 +594,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -608,9 +614,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -619,18 +625,18 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -639,18 +645,18 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -659,18 +665,18 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -679,18 +685,18 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -699,19 +705,18 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E12">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -720,17 +725,16 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -747,10 +751,10 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -767,127 +771,529 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
         <v>30</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>100</v>
       </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17">
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
         <v>40</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>90</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>100</v>
-      </c>
-      <c r="E18">
-        <v>30</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E19">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>60</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>60</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26">
         <v>30</v>
       </c>
-      <c r="E20">
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+      <c r="E28">
         <v>100</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>90</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>60</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>90</v>
+      </c>
+      <c r="E35">
         <v>40</v>
       </c>
-      <c r="E21">
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>40</v>
+      </c>
+      <c r="E37">
         <v>90</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F37" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>60</v>
+      </c>
+      <c r="E38">
+        <v>50</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>60</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>60</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed catch trials from 24 to 8
</commit_message>
<xml_diff>
--- a/design_choice_only/stim_crit.xlsx
+++ b/design_choice_only/stim_crit.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/ce_rating/design_choice_only/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E914538E-EF5D-A847-B5E4-38339E67C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD230BA-3080-9541-9469-4932BEFE71D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="500" windowWidth="24640" windowHeight="15100" xr2:uid="{83BDC93F-3B75-2E41-8B80-1829027D4291}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>t_high</t>
   </si>
@@ -56,18 +57,6 @@
     <t>effect</t>
   </si>
   <si>
-    <t>repulsion_1</t>
-  </si>
-  <si>
-    <t>repulsion_2</t>
-  </si>
-  <si>
-    <t>attraction_1</t>
-  </si>
-  <si>
-    <t>attraction_2</t>
-  </si>
-  <si>
     <t>d1</t>
   </si>
   <si>
@@ -81,6 +70,21 @@
   </si>
   <si>
     <t>binary</t>
+  </si>
+  <si>
+    <t>attraction</t>
+  </si>
+  <si>
+    <t>repulsion</t>
+  </si>
+  <si>
+    <t>repulsion_A</t>
+  </si>
+  <si>
+    <t>repulsion_B</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -466,17 +470,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D09608-67B5-B54A-8956-53E291167A46}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A41"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -485,18 +489,18 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -511,12 +515,12 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -531,112 +535,113 @@
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>100</v>
       </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="E8">
         <v>30</v>
       </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>90</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>60</v>
-      </c>
-      <c r="E8">
-        <v>50</v>
-      </c>
       <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -645,18 +650,19 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -665,18 +671,18 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E10">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -685,18 +691,18 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -705,18 +711,18 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -725,24 +731,24 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -751,18 +757,18 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>90</v>
@@ -771,12 +777,12 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -785,24 +791,24 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E16">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -811,18 +817,18 @@
         <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>40</v>
@@ -831,13 +837,12 @@
         <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -846,19 +851,18 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -873,12 +877,12 @@
         <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -893,12 +897,12 @@
         <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -913,12 +917,12 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -933,12 +937,12 @@
         <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -953,12 +957,12 @@
         <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -973,331 +977,26 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>100</v>
-      </c>
-      <c r="E26">
-        <v>30</v>
-      </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>90</v>
-      </c>
-      <c r="E27">
-        <v>40</v>
-      </c>
-      <c r="F27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-      <c r="E28">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>40</v>
-      </c>
-      <c r="E29">
-        <v>90</v>
-      </c>
-      <c r="F29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>60</v>
-      </c>
-      <c r="E30">
-        <v>50</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>50</v>
-      </c>
-      <c r="E31">
-        <v>60</v>
-      </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>50</v>
-      </c>
-      <c r="E32">
-        <v>60</v>
-      </c>
-      <c r="F32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33">
-        <v>60</v>
-      </c>
-      <c r="E33">
-        <v>50</v>
-      </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>100</v>
-      </c>
-      <c r="E34">
-        <v>30</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <v>90</v>
-      </c>
-      <c r="E35">
-        <v>40</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>30</v>
-      </c>
-      <c r="E36">
-        <v>100</v>
-      </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>40</v>
-      </c>
-      <c r="E37">
-        <v>90</v>
-      </c>
-      <c r="F37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>60</v>
-      </c>
-      <c r="E38">
-        <v>50</v>
-      </c>
-      <c r="F38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39">
-        <v>50</v>
-      </c>
-      <c r="E39">
-        <v>60</v>
-      </c>
-      <c r="F39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>50</v>
-      </c>
-      <c r="E40">
-        <v>60</v>
-      </c>
-      <c r="F40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41">
-        <v>60</v>
-      </c>
-      <c r="E41">
-        <v>50</v>
-      </c>
-      <c r="F41" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5AA75B-FF99-6D4B-A2C2-D6B3D4452189}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>